<commit_message>
Updated the Booking Reporting SSP for accepting a single Booking Report.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReportMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="1340" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="-25560" yWindow="6880" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -439,174 +439,21 @@
     <t>A text description of a residence</t>
   </si>
   <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:DocumentCreationDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:DocumentIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/intel:SystemIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/intel:SystemIdentification/nc:SystemName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonEthnicityCode</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonRaceCode</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSSNIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]nc:PersonName/nc:PersonMiddleName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/j:BailBondAmount/nc:Amount</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/nc:ActivityCategoryText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Booking[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:BookingDetentionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/cyfs:NextCourtEvent[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:CourtEventCourt/j:CourtName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/cyfs:NextCourtEvent[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Charge[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeSequenceID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Charge[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Charge[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> /br-doc:BookingReports/br-ext:BookingReport/j:Charge[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeCategoryDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Charge[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeHighestIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:DetentiontImmigrationHoldIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionAreaIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionBedIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCellIdentification/nc:IdentificationID</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonResidentText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/br-ext:PersonSocioEconomicStatusDescriptionText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/nc:EmployeeOccupationCategoryText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonMilitarySummary/nc:MilitaryExperienceIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonEducationLevelText</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/nc:ActivityStatus/nc:StatusDescriptionText</t>
-  </si>
-  <si>
     <t>Booking Date/Time</t>
   </si>
   <si>
-    <r>
-      <t>/br-doc:BookingReports/br-ext:BookingReport/j:Booking[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Time</t>
-    </r>
-  </si>
-  <si>
     <t>Arrest Location</t>
   </si>
   <si>
     <t>Arrest</t>
   </si>
   <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Location[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Address/nc:AddressFullText</t>
-  </si>
-  <si>
     <t>Release Date/Time</t>
   </si>
   <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/j:Detention[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:DateTime</t>
-  </si>
-  <si>
-    <t>br-doc:BookingReports/br-ext:BookingReport/j:Arrest/j:ArrestAgency/nc:OrganizationName</t>
-  </si>
-  <si>
-    <t>br-doc:BookingReports/br-ext:BookingReport/j:Detention/nc:SupervisionCustodyStatus/nc:StatusDescriptionText</t>
-  </si>
-  <si>
     <t>x-ext-code</t>
   </si>
   <si>
-    <t>br-doc:BookingReports/br-ext:BookingReport/j:Detention/j:SupervisionAugmentation/j:SupervisionBedIdentification/ac-bkg-codes:BedCategoryCode</t>
-  </si>
-  <si>
-    <t>br-doc:BookingReports/br-ext:BookingReport/j:Detention/nc:SupervisionCustodyStatus/ac-bkg-codes:PreTrialCategoryCode</t>
-  </si>
-  <si>
-    <t>br-doc:BookingReports/br-ext:BookingReport/j:Detention/br-ext:InmateWorkReleaseIndicator</t>
-  </si>
-  <si>
-    <t>br-doc:BookingReports/br-ext:BookingReport/j:Detention/br-ext:InmateWorkerIndicator</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonCriminalHistorySummary/j:RegisteredSexualOffenderIndicator</t>
-  </si>
-  <si>
     <t>Person Primary Language</t>
   </si>
   <si>
@@ -625,16 +472,157 @@
     <t>Case Court Name</t>
   </si>
   <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Person[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonPrimaryLanguage/nc:LanguageName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Case[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:CaseAugmentation/j:CaseCourt/j:CourtName</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Location[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLatitude/nc:LatitudeDegreeValue</t>
-  </si>
-  <si>
-    <t>/br-doc:BookingReports/br-ext:BookingReport/nc:Location[@structures:id=/br-doc:BookingReports/br-ext:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLongitude/nc:LongitudeDegreeValue</t>
+    <t>/br-doc:BookingReport/nc:DocumentCreationDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:DocumentIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/intel:SystemIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/intel:SystemIdentification/nc:SystemName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Case[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:CaseAugmentation/j:CaseCourt/j:CourtName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonBirthDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonEthnicityCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonSSNIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonStateFingerprintIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonGivenName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]nc:PersonName/nc:PersonMiddleName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonName/nc:PersonSurName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonSexCode</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonResidentText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/br-ext:PersonSocioEconomicStatusDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonAugmentation/nc:EmployeeOccupationCategoryText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonMilitarySummary/nc:MilitaryExperienceIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/j:PersonCriminalHistorySummary/j:RegisteredSexualOffenderIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonEducationLevelText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Person[@structures:id=/br-doc:BookingReport/j:Booking/j:BookingSubject/nc:RoleOfPerson/@structures:ref]/nc:PersonPrimaryLanguage/nc:LanguageName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/j:BailBondAmount/nc:Amount</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/nc:ActivityCategoryText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:BailBond[@structures:id=/br-doc:BookingReport/j:BailBondChargeAssociation/j:BailBond/@structures:ref]/nc:ActivityStatus/nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking/j:BookingSubject/j:SubjectIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Booking[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:BookingDetentionFacility/nc:FacilityIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/cyfs:NextCourtEvent[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:CourtEventCourt/j:CourtName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/cyfs:NextCourtEvent[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeSequenceID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeStatute/j:StatuteCodeSectionIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeCategoryDescriptionText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Charge[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/j:Charge/@structures:ref]/j:ChargeHighestIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Location[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Address/nc:AddressFullText</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Location[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLatitude/nc:LatitudeDegreeValue</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/nc:Location[@structures:id=/br-doc:BookingReport/j:Arrest/j:ArrestLocation/@structures:ref]/nc:Location2DGeospatialCoordinate/nc:GeographicCoordinateLongitude/nc:LongitudeDegreeValue</t>
+  </si>
+  <si>
+    <t>br-doc:BookingReport/j:Arrest/j:ArrestAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:DateTime</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/nc:ActivityDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:HoldForAgency/nc:OrganizationName</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/br-ext:DetentiontImmigrationHoldIndicator</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionReleaseDate/nc:Date</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionAreaIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionBedIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/br-doc:BookingReport/j:Detention[@structures:id=/br-doc:BookingReport/j:ActivityChargeAssociation/nc:Activity/@structures:ref]/j:SupervisionAugmentation/j:SupervisionCellIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>br-doc:BookingReport/j:Detention/j:SupervisionAugmentation/j:SupervisionBedIdentification/ac-bkg-codes:BedCategoryCode</t>
+  </si>
+  <si>
+    <t>br-doc:BookingReport/j:Detention/nc:SupervisionCustodyStatus/ac-bkg-codes:PreTrialCategoryCode</t>
+  </si>
+  <si>
+    <t>br-doc:BookingReport/j:Detention/nc:SupervisionCustodyStatus/nc:StatusDescriptionText</t>
+  </si>
+  <si>
+    <t>br-doc:BookingReport/j:Detention/br-ext:InmateWorkReleaseIndicator</t>
+  </si>
+  <si>
+    <t>br-doc:BookingReport/j:Detention/br-ext:InmateWorkerIndicator</t>
   </si>
 </sst>
 </file>
@@ -2695,8 +2683,8 @@
   <dimension ref="A1:L385"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="D48"/>
+      <pane ySplit="2" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2726,7 +2714,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:12" ht="47.25">
+    <row r="2" spans="1:12" ht="45">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -2780,7 +2768,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="31.5">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>7</v>
@@ -2790,7 +2778,7 @@
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>10</v>
@@ -2812,7 +2800,7 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>10</v>
@@ -2850,7 +2838,7 @@
       </c>
       <c r="D7" s="17"/>
       <c r="E7" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -2872,7 +2860,7 @@
       </c>
       <c r="D8" s="17"/>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2886,7 +2874,7 @@
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="6" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2903,12 +2891,12 @@
     <row r="10" spans="1:12" ht="45">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>181</v>
+        <v>134</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="18" t="s">
-        <v>183</v>
+        <v>139</v>
       </c>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
@@ -2933,7 +2921,7 @@
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
     </row>
-    <row r="12" spans="1:12" ht="31.5">
+    <row r="12" spans="1:12" ht="30">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
         <v>14</v>
@@ -2943,7 +2931,7 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="18" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>21</v>
@@ -2962,7 +2950,7 @@
       </c>
       <c r="K12" s="24"/>
     </row>
-    <row r="13" spans="1:12" ht="31.5">
+    <row r="13" spans="1:12" ht="30">
       <c r="A13" s="9"/>
       <c r="B13" s="9" t="s">
         <v>2</v>
@@ -2972,7 +2960,7 @@
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="18" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
@@ -2987,7 +2975,7 @@
       </c>
       <c r="K13" s="24"/>
     </row>
-    <row r="14" spans="1:12" ht="31.5">
+    <row r="14" spans="1:12" ht="30">
       <c r="A14" s="9"/>
       <c r="B14" s="9" t="s">
         <v>0</v>
@@ -2997,7 +2985,7 @@
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="18" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="8" t="s">
@@ -3014,7 +3002,7 @@
       </c>
       <c r="K14" s="24"/>
     </row>
-    <row r="15" spans="1:12" ht="47.25">
+    <row r="15" spans="1:12" ht="45">
       <c r="A15" s="9"/>
       <c r="B15" s="9" t="s">
         <v>54</v>
@@ -3024,7 +3012,7 @@
       </c>
       <c r="D15" s="8"/>
       <c r="E15" s="19" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
@@ -3044,7 +3032,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="47.25">
+    <row r="16" spans="1:12" ht="45">
       <c r="A16" s="9"/>
       <c r="B16" s="9" t="s">
         <v>57</v>
@@ -3054,7 +3042,7 @@
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="19" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="18" t="s">
@@ -3074,7 +3062,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="47.25">
+    <row r="17" spans="1:12" ht="45">
       <c r="A17" s="9"/>
       <c r="B17" s="9" t="s">
         <v>61</v>
@@ -3084,7 +3072,7 @@
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="19" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>21</v>
@@ -3106,7 +3094,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="47.25">
+    <row r="18" spans="1:12" ht="45">
       <c r="A18" s="9"/>
       <c r="B18" s="9" t="s">
         <v>62</v>
@@ -3116,7 +3104,7 @@
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="19" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="F18" s="18" t="s">
         <v>21</v>
@@ -3138,7 +3126,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="47.25">
+    <row r="19" spans="1:12" ht="45">
       <c r="A19" s="9"/>
       <c r="B19" s="9" t="s">
         <v>63</v>
@@ -3148,7 +3136,7 @@
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="19" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>21</v>
@@ -3170,7 +3158,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="31.5">
+    <row r="20" spans="1:12" ht="30">
       <c r="A20" s="9"/>
       <c r="B20" s="9" t="s">
         <v>1</v>
@@ -3180,7 +3168,7 @@
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>21</v>
@@ -3197,7 +3185,7 @@
       </c>
       <c r="K20" s="24"/>
     </row>
-    <row r="21" spans="1:12" ht="31.5">
+    <row r="21" spans="1:12" ht="30">
       <c r="A21" s="10"/>
       <c r="B21" s="10" t="s">
         <v>121</v>
@@ -3207,7 +3195,7 @@
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="30" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11"/>
@@ -3221,7 +3209,7 @@
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
     </row>
-    <row r="22" spans="1:12" ht="47.25">
+    <row r="22" spans="1:12" ht="45">
       <c r="A22" s="10" t="s">
         <v>44</v>
       </c>
@@ -3233,7 +3221,7 @@
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="30" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="11"/>
@@ -3247,7 +3235,7 @@
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
     </row>
-    <row r="23" spans="1:12" ht="47.25">
+    <row r="23" spans="1:12" ht="45">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="s">
         <v>102</v>
@@ -3257,7 +3245,7 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="30" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="11"/>
@@ -3271,7 +3259,7 @@
       <c r="K23" s="33"/>
       <c r="L23" s="33"/>
     </row>
-    <row r="24" spans="1:12" ht="47.25">
+    <row r="24" spans="1:12" ht="45">
       <c r="A24" s="10"/>
       <c r="B24" s="10" t="s">
         <v>103</v>
@@ -3281,7 +3269,7 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="30" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
@@ -3305,7 +3293,7 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="30" t="s">
-        <v>175</v>
+        <v>153</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
@@ -3319,7 +3307,7 @@
       <c r="K25" s="33"/>
       <c r="L25" s="33"/>
     </row>
-    <row r="26" spans="1:12" ht="47.25">
+    <row r="26" spans="1:12" ht="30">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="s">
         <v>101</v>
@@ -3329,7 +3317,7 @@
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="30" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F26" s="11"/>
       <c r="G26" s="11"/>
@@ -3346,12 +3334,12 @@
     <row r="27" spans="1:12" ht="45">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="28"/>
       <c r="E27" s="30" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="F27" s="11"/>
       <c r="G27" s="11"/>
@@ -3377,7 +3365,7 @@
       <c r="K28" s="7"/>
       <c r="L28" s="7"/>
     </row>
-    <row r="29" spans="1:12" ht="31.5">
+    <row r="29" spans="1:12" ht="30">
       <c r="A29" s="13"/>
       <c r="B29" s="10" t="s">
         <v>18</v>
@@ -3386,7 +3374,7 @@
         <v>36</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>21</v>
@@ -3400,7 +3388,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="31.5">
+    <row r="30" spans="1:12" ht="30">
       <c r="A30" s="13"/>
       <c r="B30" s="10" t="s">
         <v>19</v>
@@ -3410,7 +3398,7 @@
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="12" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>21</v>
@@ -3424,7 +3412,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="78.75">
+    <row r="31" spans="1:12" ht="75">
       <c r="A31" s="34"/>
       <c r="B31" s="35" t="s">
         <v>79</v>
@@ -3434,7 +3422,7 @@
       </c>
       <c r="D31" s="35"/>
       <c r="E31" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F31" s="33"/>
       <c r="G31" s="36"/>
@@ -3466,7 +3454,7 @@
       <c r="K32" s="7"/>
       <c r="L32" s="7"/>
     </row>
-    <row r="33" spans="1:12" s="14" customFormat="1" ht="31.5">
+    <row r="33" spans="1:12" s="14" customFormat="1" ht="30">
       <c r="B33" s="16" t="s">
         <v>53</v>
       </c>
@@ -3475,7 +3463,7 @@
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="13" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="F33" s="22" t="s">
         <v>21</v>
@@ -3493,17 +3481,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="31.5">
+    <row r="34" spans="1:12" ht="30">
       <c r="A34" s="8"/>
       <c r="B34" s="9" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>160</v>
+        <v>124</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F34" s="8" t="s">
         <v>21</v>
@@ -3519,7 +3507,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="47.25">
+    <row r="35" spans="1:12" ht="45">
       <c r="A35" s="8"/>
       <c r="B35" s="9" t="s">
         <v>22</v>
@@ -3529,7 +3517,7 @@
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="12" t="s">
-        <v>140</v>
+        <v>161</v>
       </c>
       <c r="F35" s="8"/>
       <c r="G35" s="8" t="s">
@@ -3557,7 +3545,7 @@
       <c r="K36" s="7"/>
       <c r="L36" s="7"/>
     </row>
-    <row r="37" spans="1:12" ht="47.25">
+    <row r="37" spans="1:12" ht="30">
       <c r="A37" s="13"/>
       <c r="B37" s="37" t="s">
         <v>109</v>
@@ -3565,7 +3553,7 @@
       <c r="C37" s="13"/>
       <c r="D37" s="13"/>
       <c r="E37" s="18" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="F37" s="13"/>
       <c r="G37" s="13"/>
@@ -3590,7 +3578,7 @@
         <v>46</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
       <c r="F38" s="11" t="s">
         <v>21</v>
@@ -3620,7 +3608,7 @@
       <c r="K39" s="7"/>
       <c r="L39" s="7"/>
     </row>
-    <row r="40" spans="1:12" ht="31.5">
+    <row r="40" spans="1:12" ht="30">
       <c r="A40" s="13"/>
       <c r="B40" s="10" t="s">
         <v>17</v>
@@ -3629,7 +3617,7 @@
         <v>47</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>143</v>
+        <v>164</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>21</v>
@@ -3643,7 +3631,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="31.5">
+    <row r="41" spans="1:12" ht="30">
       <c r="A41" s="13"/>
       <c r="B41" s="10" t="s">
         <v>9</v>
@@ -3652,7 +3640,7 @@
         <v>37</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>144</v>
+        <v>165</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>21</v>
@@ -3666,7 +3654,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="47.25">
+    <row r="42" spans="1:12" ht="45">
       <c r="A42" s="13"/>
       <c r="B42" s="10" t="s">
         <v>108</v>
@@ -3675,7 +3663,7 @@
         <v>48</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>21</v>
@@ -3689,7 +3677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="173.25">
+    <row r="43" spans="1:12" ht="165">
       <c r="A43" s="34"/>
       <c r="B43" s="35" t="s">
         <v>88</v>
@@ -3699,7 +3687,7 @@
       </c>
       <c r="D43" s="32"/>
       <c r="E43" s="35" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="F43" s="11"/>
       <c r="G43" s="36"/>
@@ -3715,7 +3703,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="31.5">
+    <row r="44" spans="1:12" ht="30">
       <c r="A44" s="20" t="s">
         <v>44</v>
       </c>
@@ -3727,7 +3715,7 @@
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="18" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
@@ -3740,7 +3728,7 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="6" t="s">
-        <v>163</v>
+        <v>126</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -3754,17 +3742,17 @@
       <c r="K45" s="7"/>
       <c r="L45" s="26"/>
     </row>
-    <row r="46" spans="1:12" ht="63">
+    <row r="46" spans="1:12" ht="60">
       <c r="A46" s="34"/>
       <c r="B46" s="39" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="C46" s="38" t="s">
         <v>117</v>
       </c>
       <c r="D46" s="32"/>
       <c r="E46" s="30" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="F46" s="33"/>
       <c r="G46" s="36"/>
@@ -3781,12 +3769,12 @@
     <row r="47" spans="1:12" ht="45">
       <c r="A47" s="34"/>
       <c r="B47" s="39" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="C47" s="38"/>
       <c r="D47" s="32"/>
       <c r="E47" s="30" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="F47" s="33"/>
       <c r="G47" s="36"/>
@@ -3799,12 +3787,12 @@
     <row r="48" spans="1:12" ht="45">
       <c r="A48" s="34"/>
       <c r="B48" s="39" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
       <c r="C48" s="38"/>
       <c r="D48" s="32"/>
       <c r="E48" s="30" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
       <c r="F48" s="33"/>
       <c r="G48" s="36"/>
@@ -3814,7 +3802,7 @@
       <c r="K48" s="33"/>
       <c r="L48" s="33"/>
     </row>
-    <row r="49" spans="1:12" ht="63">
+    <row r="49" spans="1:12" ht="60">
       <c r="A49" s="36"/>
       <c r="B49" s="38" t="s">
         <v>87</v>
@@ -3824,7 +3812,7 @@
       </c>
       <c r="D49" s="32"/>
       <c r="E49" s="30" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F49" s="11"/>
       <c r="G49" s="36"/>
@@ -3850,16 +3838,16 @@
       <c r="K50" s="7"/>
       <c r="L50" s="26"/>
     </row>
-    <row r="51" spans="1:12" ht="47.25">
+    <row r="51" spans="1:12" ht="45">
       <c r="A51" s="13"/>
       <c r="B51" s="10" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>38</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="F51" s="13"/>
       <c r="G51" s="13" t="s">
@@ -3875,7 +3863,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="31.5">
+    <row r="52" spans="1:12" ht="30">
       <c r="A52" s="13"/>
       <c r="B52" s="10" t="s">
         <v>23</v>
@@ -3884,7 +3872,7 @@
         <v>39</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="F52" s="13"/>
       <c r="G52" s="13" t="s">
@@ -3901,7 +3889,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="47.25">
+    <row r="53" spans="1:12" ht="45">
       <c r="A53" s="13" t="s">
         <v>44</v>
       </c>
@@ -3913,7 +3901,7 @@
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="17" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="F53" s="11" t="s">
         <v>21</v>
@@ -3930,7 +3918,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="47.25">
+    <row r="54" spans="1:12" ht="45">
       <c r="A54" s="13" t="s">
         <v>44</v>
       </c>
@@ -3941,7 +3929,7 @@
         <v>49</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="F54" s="11" t="s">
         <v>21</v>
@@ -3955,7 +3943,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="47.25">
+    <row r="55" spans="1:12" ht="45">
       <c r="B55" s="10" t="s">
         <v>42</v>
       </c>
@@ -3963,7 +3951,7 @@
         <v>41</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="F55" s="11" t="s">
         <v>21</v>
@@ -3982,7 +3970,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="47.25">
+    <row r="56" spans="1:12" ht="45">
       <c r="A56" s="13"/>
       <c r="B56" s="9" t="s">
         <v>64</v>
@@ -3992,7 +3980,7 @@
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="12" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="F56" s="13"/>
       <c r="G56" s="20" t="s">
@@ -4004,7 +3992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="47.25">
+    <row r="57" spans="1:12" ht="45">
       <c r="A57" s="13"/>
       <c r="B57" s="9" t="s">
         <v>65</v>
@@ -4014,7 +4002,7 @@
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="12" t="s">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="F57" s="13"/>
       <c r="G57" s="20" t="s">
@@ -4026,7 +4014,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="47.25">
+    <row r="58" spans="1:12" ht="45">
       <c r="A58" s="13"/>
       <c r="B58" s="4" t="s">
         <v>66</v>
@@ -4036,7 +4024,7 @@
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="12" t="s">
-        <v>153</v>
+        <v>180</v>
       </c>
       <c r="F58" s="13"/>
       <c r="G58" s="20" t="s">
@@ -4048,9 +4036,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="47.25">
+    <row r="59" spans="1:12" ht="45">
       <c r="A59" s="20" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="B59" s="20" t="s">
         <v>72</v>
@@ -4060,7 +4048,7 @@
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="17" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F59" s="13"/>
       <c r="G59" s="13"/>
@@ -4072,17 +4060,17 @@
     </row>
     <row r="60" spans="1:12" ht="30">
       <c r="A60" s="20" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="17" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
@@ -4094,7 +4082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="31.5">
+    <row r="61" spans="1:12" ht="30">
       <c r="A61" s="34"/>
       <c r="B61" s="38" t="s">
         <v>91</v>
@@ -4104,7 +4092,7 @@
       </c>
       <c r="D61" s="32"/>
       <c r="E61" s="40" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="F61" s="36"/>
       <c r="G61" s="36"/>
@@ -4120,7 +4108,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="31.5">
+    <row r="62" spans="1:12" ht="30">
       <c r="A62" s="34" t="s">
         <v>44</v>
       </c>
@@ -4132,7 +4120,7 @@
       </c>
       <c r="D62" s="32"/>
       <c r="E62" s="42" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="F62" s="36"/>
       <c r="G62" s="36"/>
@@ -4146,7 +4134,7 @@
       <c r="K62" s="33"/>
       <c r="L62" s="33"/>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" ht="30">
       <c r="A63" s="34" t="s">
         <v>44</v>
       </c>
@@ -4158,7 +4146,7 @@
       </c>
       <c r="D63" s="32"/>
       <c r="E63" s="42" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F63" s="36"/>
       <c r="G63" s="36"/>
@@ -4203,7 +4191,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" ht="63">
+    <row r="67" spans="1:9" ht="60">
       <c r="A67" s="20"/>
       <c r="B67" s="20" t="s">
         <v>85</v>
@@ -6072,7 +6060,7 @@
       <c r="H273" s="13"/>
       <c r="I273" s="13"/>
     </row>
-    <row r="274" spans="1:9" ht="15.75" hidden="1">
+    <row r="274" spans="1:9" hidden="1">
       <c r="A274" s="13"/>
       <c r="B274" s="13"/>
       <c r="E274" s="13"/>
@@ -6081,7 +6069,7 @@
       <c r="H274" s="13"/>
       <c r="I274" s="13"/>
     </row>
-    <row r="275" spans="1:9" ht="15.75" hidden="1">
+    <row r="275" spans="1:9" hidden="1">
       <c r="A275" s="13"/>
       <c r="B275" s="13"/>
       <c r="E275" s="13"/>
@@ -6090,7 +6078,7 @@
       <c r="H275" s="13"/>
       <c r="I275" s="13"/>
     </row>
-    <row r="276" spans="1:9" ht="15.75" hidden="1">
+    <row r="276" spans="1:9" hidden="1">
       <c r="A276" s="13"/>
       <c r="B276" s="13"/>
       <c r="E276" s="13"/>
@@ -6099,7 +6087,7 @@
       <c r="H276" s="13"/>
       <c r="I276" s="13"/>
     </row>
-    <row r="277" spans="1:9" ht="15.75" hidden="1">
+    <row r="277" spans="1:9" hidden="1">
       <c r="A277" s="13"/>
       <c r="B277" s="13"/>
       <c r="E277" s="13"/>
@@ -6108,7 +6096,7 @@
       <c r="H277" s="13"/>
       <c r="I277" s="13"/>
     </row>
-    <row r="278" spans="1:9" ht="15.75" hidden="1">
+    <row r="278" spans="1:9" hidden="1">
       <c r="A278" s="13"/>
       <c r="B278" s="13"/>
       <c r="E278" s="13"/>
@@ -6117,7 +6105,7 @@
       <c r="H278" s="13"/>
       <c r="I278" s="13"/>
     </row>
-    <row r="279" spans="1:9" ht="15.75" hidden="1">
+    <row r="279" spans="1:9" hidden="1">
       <c r="A279" s="13"/>
       <c r="B279" s="13"/>
       <c r="E279" s="13"/>
@@ -6126,7 +6114,7 @@
       <c r="H279" s="13"/>
       <c r="I279" s="13"/>
     </row>
-    <row r="280" spans="1:9" ht="15.75" hidden="1">
+    <row r="280" spans="1:9" hidden="1">
       <c r="A280" s="13"/>
       <c r="B280" s="13"/>
       <c r="E280" s="13"/>
@@ -6135,7 +6123,7 @@
       <c r="H280" s="13"/>
       <c r="I280" s="13"/>
     </row>
-    <row r="281" spans="1:9" ht="15.75" hidden="1">
+    <row r="281" spans="1:9" hidden="1">
       <c r="A281" s="13"/>
       <c r="B281" s="13"/>
       <c r="E281" s="13"/>
@@ -6144,7 +6132,7 @@
       <c r="H281" s="13"/>
       <c r="I281" s="13"/>
     </row>
-    <row r="282" spans="1:9" ht="15.75" hidden="1">
+    <row r="282" spans="1:9" hidden="1">
       <c r="A282" s="13"/>
       <c r="B282" s="13"/>
       <c r="E282" s="13"/>
@@ -6153,7 +6141,7 @@
       <c r="H282" s="13"/>
       <c r="I282" s="13"/>
     </row>
-    <row r="283" spans="1:9" ht="15.75" hidden="1">
+    <row r="283" spans="1:9" hidden="1">
       <c r="A283" s="13"/>
       <c r="B283" s="13"/>
       <c r="E283" s="13"/>
@@ -6162,7 +6150,7 @@
       <c r="H283" s="13"/>
       <c r="I283" s="13"/>
     </row>
-    <row r="284" spans="1:9" ht="15.75" hidden="1">
+    <row r="284" spans="1:9" hidden="1">
       <c r="A284" s="13"/>
       <c r="B284" s="13"/>
       <c r="E284" s="13"/>
@@ -6171,7 +6159,7 @@
       <c r="H284" s="13"/>
       <c r="I284" s="13"/>
     </row>
-    <row r="285" spans="1:9" ht="15.75" hidden="1">
+    <row r="285" spans="1:9" hidden="1">
       <c r="A285" s="13"/>
       <c r="B285" s="13"/>
       <c r="E285" s="13"/>
@@ -6180,7 +6168,7 @@
       <c r="H285" s="13"/>
       <c r="I285" s="13"/>
     </row>
-    <row r="286" spans="1:9" ht="15.75" hidden="1">
+    <row r="286" spans="1:9" hidden="1">
       <c r="A286" s="13"/>
       <c r="B286" s="13"/>
       <c r="E286" s="13"/>
@@ -6189,7 +6177,7 @@
       <c r="H286" s="13"/>
       <c r="I286" s="13"/>
     </row>
-    <row r="287" spans="1:9" ht="15.75" hidden="1">
+    <row r="287" spans="1:9" hidden="1">
       <c r="A287" s="13"/>
       <c r="B287" s="13"/>
       <c r="E287" s="13"/>

</xml_diff>

<commit_message>
Added new elements to "Custody" SSPs.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReportMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9020" yWindow="3680" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="940" yWindow="1080" windowWidth="31400" windowHeight="17440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Booking Report" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="215">
   <si>
     <t>Race</t>
   </si>
@@ -616,13 +616,61 @@
   </si>
   <si>
     <t xml:space="preserve"> The agency for whom a subject is being held. (sending agency)</t>
+  </si>
+  <si>
+    <t>Eye Color</t>
+  </si>
+  <si>
+    <t>Hair Color</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Physical Feature Desc.</t>
+  </si>
+  <si>
+    <t>Scars, Marks, Tattoos</t>
+  </si>
+  <si>
+    <t>Allow Account Deposit Indicator</t>
+  </si>
+  <si>
+    <t>Supervision Conditions</t>
+  </si>
+  <si>
+    <t>Propbation/Parole Officer</t>
+  </si>
+  <si>
+    <t>Fullname</t>
+  </si>
+  <si>
+    <t>Supervisor Category</t>
+  </si>
+  <si>
+    <t>Supervisor Status</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Phone Category Desc.</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Age</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -690,8 +738,29 @@
       <sz val="11"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -712,6 +781,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -740,7 +815,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="762">
+  <cellStyleXfs count="766">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1503,8 +1578,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1540,9 +1619,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1585,8 +1661,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="762">
+  <cellStyles count="766">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1967,6 +2070,8 @@
     <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2347,6 +2452,8 @@
     <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2682,17 +2789,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L387"/>
+  <dimension ref="A1:L402"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD83"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83:XFD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="2" customWidth="1"/>
     <col min="3" max="4" width="28.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="92.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" style="2" customWidth="1"/>
@@ -2705,10 +2812,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="27"/>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
       <c r="E1" s="1"/>
@@ -2770,7 +2877,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" s="14" customFormat="1" ht="30">
+    <row r="4" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A4" s="6"/>
       <c r="B4" s="6" t="s">
         <v>7</v>
@@ -2792,7 +2899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="14" customFormat="1">
+    <row r="5" spans="1:12" s="13" customFormat="1">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
         <v>5</v>
@@ -2814,83 +2921,83 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="14" customFormat="1">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:12" s="13" customFormat="1">
+      <c r="A6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-    </row>
-    <row r="7" spans="1:12" s="14" customFormat="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+    </row>
+    <row r="7" spans="1:12" s="13" customFormat="1">
+      <c r="A7" s="16"/>
+      <c r="B7" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="17"/>
+      <c r="E7" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="14" customFormat="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17" t="s">
+    <row r="8" spans="1:12" s="13" customFormat="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="17" t="s">
+      <c r="D8" s="17"/>
+      <c r="E8" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="14" customFormat="1">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:12" s="13" customFormat="1">
+      <c r="A9" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-    </row>
-    <row r="10" spans="1:12" s="14" customFormat="1" ht="45">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+    </row>
+    <row r="10" spans="1:12" s="13" customFormat="1" ht="45">
       <c r="A10" s="6"/>
       <c r="B10" s="6" t="s">
         <v>131</v>
@@ -2904,24 +3011,24 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:12" s="14" customFormat="1">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:12" s="13" customFormat="1">
+      <c r="A11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" spans="1:12" s="12" customFormat="1" ht="45">
-      <c r="A12" s="19"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="7" t="s">
         <v>184</v>
       </c>
@@ -2938,186 +3045,115 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K16" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L17" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="20" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" s="14" customFormat="1" ht="45">
+    <row r="13" spans="1:12" s="30" customFormat="1">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+    </row>
+    <row r="14" spans="1:12" s="30" customFormat="1">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29" t="s">
+        <v>199</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+    </row>
+    <row r="15" spans="1:12" s="30" customFormat="1">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+    </row>
+    <row r="16" spans="1:12" s="30" customFormat="1">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="1:12" s="30" customFormat="1">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+    </row>
+    <row r="18" spans="1:12" s="30" customFormat="1">
+      <c r="A18" s="28"/>
+      <c r="B18" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+    </row>
+    <row r="19" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A19" s="6"/>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="20" t="s">
-        <v>143</v>
+      <c r="E19" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>21</v>
@@ -3128,1478 +3164,1616 @@
       <c r="H19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" s="14" customFormat="1" ht="45">
+      <c r="I19" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
-        <v>63</v>
+        <v>2</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="20" t="s">
-        <v>144</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="E20" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
       <c r="H20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="14" customFormat="1" ht="30">
+      <c r="I20" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A21" s="6"/>
       <c r="B21" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>188</v>
+        <v>35</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-    </row>
-    <row r="23" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A23" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-    </row>
-    <row r="24" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="J24" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-    </row>
-    <row r="25" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-    </row>
-    <row r="26" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-    </row>
-    <row r="27" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-    </row>
-    <row r="28" spans="1:12" s="14" customFormat="1" ht="45">
+      <c r="F27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A28" s="7"/>
       <c r="B28" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
+        <v>118</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28" s="20"/>
       <c r="E28" s="7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="12"/>
+      <c r="I28" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>21</v>
+      </c>
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" s="14" customFormat="1">
-      <c r="A29" s="15" t="s">
+    <row r="29" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+    </row>
+    <row r="30" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+    </row>
+    <row r="31" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+    </row>
+    <row r="32" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+    </row>
+    <row r="33" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+    </row>
+    <row r="34" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+    </row>
+    <row r="35" spans="1:12" s="13" customFormat="1">
+      <c r="A35" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="16"/>
-    </row>
-    <row r="30" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6" t="s">
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+    </row>
+    <row r="36" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="23" t="s">
+      <c r="D36" s="6"/>
+      <c r="E36" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J30" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6" t="s">
+      <c r="F36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="23" t="s">
+      <c r="D37" s="6"/>
+      <c r="E37" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="14" t="s">
+      <c r="F37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6" t="s">
+    <row r="38" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="23" t="s">
+      <c r="D38" s="6"/>
+      <c r="E38" s="22" t="s">
         <v>193</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J32" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L32" s="14" t="s">
+      <c r="F38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6" t="s">
+    <row r="39" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="23" t="s">
+      <c r="D39" s="6"/>
+      <c r="E39" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J33" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L33" s="14" t="s">
+      <c r="F39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6" t="s">
+    <row r="40" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="23" t="s">
+      <c r="D40" s="6"/>
+      <c r="E40" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J34" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="14" customFormat="1">
-      <c r="A35" s="15" t="s">
+      <c r="F40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="13" customFormat="1">
+      <c r="A41" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="16"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
-    </row>
-    <row r="36" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A36" s="11"/>
-      <c r="B36" s="7" t="s">
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+    </row>
+    <row r="42" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A42" s="11"/>
+      <c r="B42" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C42" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J36" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A37" s="11"/>
-      <c r="B37" s="7" t="s">
+      <c r="F42" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A43" s="11"/>
+      <c r="B43" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C43" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="E37" s="6" t="s">
+      <c r="E43" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J37" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="14" customFormat="1" ht="75">
-      <c r="A38" s="22"/>
-      <c r="B38" s="12" t="s">
+      <c r="F43" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="13" customFormat="1" ht="75">
+      <c r="A44" s="21"/>
+      <c r="B44" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C44" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="6" t="s">
+      <c r="D44" s="12"/>
+      <c r="E44" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K38" s="12"/>
-      <c r="L38" s="12" t="s">
+      <c r="F44" s="12"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J44" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="12"/>
+      <c r="L44" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="14" customFormat="1">
-      <c r="A39" s="15" t="s">
+    <row r="45" spans="1:12" s="13" customFormat="1">
+      <c r="A45" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="16"/>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16"/>
-    </row>
-    <row r="40" spans="1:12" s="17" customFormat="1" ht="30">
-      <c r="B40" s="24" t="s">
+      <c r="B45" s="15"/>
+      <c r="C45" s="15"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="15"/>
+      <c r="L45" s="15"/>
+    </row>
+    <row r="46" spans="1:12" s="16" customFormat="1" ht="30">
+      <c r="B46" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C40" s="18" t="s">
+      <c r="C46" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="D40" s="18"/>
-      <c r="E40" s="11" t="s">
+      <c r="D46" s="17"/>
+      <c r="E46" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="F40" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="G40" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="I40" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J40" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6" t="s">
+      <c r="F46" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="G46" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6" t="s">
+      <c r="D47" s="6"/>
+      <c r="E47" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I41" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J41" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6" t="s">
+      <c r="F47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6" t="s">
+      <c r="D48" s="6"/>
+      <c r="E48" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" s="6"/>
-      <c r="J42" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="14" customFormat="1">
-      <c r="A43" s="15" t="s">
+      <c r="F48" s="6"/>
+      <c r="G48" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" s="6"/>
+      <c r="J48" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="13" customFormat="1">
+      <c r="A49" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="16"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="16"/>
-      <c r="J43" s="16"/>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16"/>
-    </row>
-    <row r="44" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A44" s="11"/>
-      <c r="B44" s="11" t="s">
+      <c r="B49" s="15"/>
+      <c r="C49" s="15"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="15"/>
+      <c r="L49" s="15"/>
+    </row>
+    <row r="50" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
-      <c r="E44" s="6" t="s">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J44" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11" t="s">
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K50" s="11"/>
+      <c r="L50" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="14" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A45" s="11"/>
-      <c r="B45" s="7" t="s">
+    <row r="51" spans="1:12" s="13" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A51" s="11"/>
+      <c r="B51" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C51" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="6" t="s">
+      <c r="E51" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="F45" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J45" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="14" customFormat="1">
-      <c r="A46" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="16"/>
-      <c r="H46" s="16"/>
-      <c r="I46" s="16"/>
-      <c r="J46" s="16"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="16"/>
-    </row>
-    <row r="47" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A47" s="11"/>
-      <c r="B47" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C47" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J47" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A48" s="11"/>
-      <c r="B48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E48" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J48" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A49" s="11"/>
-      <c r="B49" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J49" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="14" customFormat="1" ht="165">
-      <c r="A50" s="22"/>
-      <c r="B50" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J50" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K50" s="12"/>
-      <c r="L50" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A51" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B51" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>165</v>
+      <c r="F51" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="G51" s="11"/>
       <c r="H51" s="11"/>
-      <c r="I51" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J51" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" s="14" customFormat="1">
-      <c r="A52" s="15" t="s">
+      <c r="I51" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J51" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" s="13" customFormat="1">
+      <c r="A52" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="15"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="15"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="15"/>
+      <c r="L52" s="15"/>
+    </row>
+    <row r="53" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A53" s="11"/>
+      <c r="B53" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A54" s="11"/>
+      <c r="B54" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A55" s="11"/>
+      <c r="B55" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J55" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" s="13" customFormat="1" ht="165">
+      <c r="A56" s="21"/>
+      <c r="B56" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K56" s="12"/>
+      <c r="L56" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A57" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" s="13" customFormat="1">
+      <c r="A58" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="16"/>
-      <c r="I52" s="16"/>
-      <c r="J52" s="16"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="16"/>
-    </row>
-    <row r="53" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A53" s="22"/>
-      <c r="B53" s="26" t="s">
+      <c r="B58" s="15"/>
+      <c r="C58" s="15"/>
+      <c r="D58" s="15"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+    </row>
+    <row r="59" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A59" s="21"/>
+      <c r="B59" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C59" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="7" t="s">
+      <c r="D59" s="12"/>
+      <c r="E59" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="F53" s="12"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="22"/>
-      <c r="I53" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J53" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K53" s="12"/>
-      <c r="L53" s="12"/>
-    </row>
-    <row r="54" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A54" s="22"/>
-      <c r="B54" s="26" t="s">
+      <c r="F59" s="12"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K59" s="12"/>
+      <c r="L59" s="12"/>
+    </row>
+    <row r="60" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A60" s="21"/>
+      <c r="B60" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="7" t="s">
+      <c r="C60" s="12"/>
+      <c r="D60" s="12"/>
+      <c r="E60" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="F54" s="12"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="12"/>
-      <c r="K54" s="12"/>
-      <c r="L54" s="12"/>
-    </row>
-    <row r="55" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A55" s="22"/>
-      <c r="B55" s="26" t="s">
+      <c r="F60" s="12"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="12"/>
+      <c r="L60" s="12"/>
+    </row>
+    <row r="61" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A61" s="21"/>
+      <c r="B61" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="7" t="s">
+      <c r="C61" s="12"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="F55" s="12"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
-      <c r="I55" s="12"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12"/>
-      <c r="L55" s="12"/>
-    </row>
-    <row r="56" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A56" s="22"/>
-      <c r="B56" s="12" t="s">
+      <c r="F61" s="12"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="12"/>
+      <c r="L61" s="12"/>
+    </row>
+    <row r="62" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A62" s="21"/>
+      <c r="B62" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="12" t="s">
+      <c r="C62" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D56" s="12"/>
-      <c r="E56" s="7" t="s">
+      <c r="D62" s="12"/>
+      <c r="E62" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="22"/>
-      <c r="J56" s="12"/>
-      <c r="K56" s="12"/>
-      <c r="L56" s="12"/>
-    </row>
-    <row r="57" spans="1:12" s="14" customFormat="1">
-      <c r="A57" s="15" t="s">
+      <c r="F62" s="7"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="12"/>
+      <c r="K62" s="12"/>
+      <c r="L62" s="12"/>
+    </row>
+    <row r="63" spans="1:12" s="13" customFormat="1">
+      <c r="A63" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B57" s="16"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="16"/>
-      <c r="I57" s="16"/>
-      <c r="J57" s="16"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="16"/>
-    </row>
-    <row r="58" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A58" s="11"/>
-      <c r="B58" s="7" t="s">
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+    </row>
+    <row r="64" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A64" s="11"/>
+      <c r="B64" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C64" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E58" s="6" t="s">
+      <c r="E64" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I58" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J58" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A59" s="11"/>
-      <c r="B59" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="J59" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="L59" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A60" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J60" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L60" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A61" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E61" s="18" t="s">
-        <v>173</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J61" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="B62" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E62" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I62" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="J62" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L62" s="14" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A63" s="11"/>
-      <c r="B63" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E63" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" s="14" customFormat="1" ht="45">
-      <c r="A64" s="11"/>
-      <c r="B64" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="F64" s="11"/>
       <c r="G64" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" s="14" customFormat="1" ht="45">
+      <c r="H64" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J64" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A65" s="11"/>
-      <c r="B65" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C65" s="14" t="s">
-        <v>70</v>
+      <c r="B65" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F65" s="11"/>
       <c r="G65" s="11" t="s">
         <v>21</v>
       </c>
       <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" s="14" customFormat="1" ht="30">
+      <c r="I65" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="J65" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="L65" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" s="13" customFormat="1" ht="45">
       <c r="A66" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B66" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="E66" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="F66" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C66" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G66" s="11"/>
       <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" s="14" customFormat="1" ht="30">
+      <c r="I66" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J66" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L66" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" s="13" customFormat="1" ht="45">
       <c r="A67" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B67" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>179</v>
-      </c>
-      <c r="F67" s="11"/>
+        <v>44</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E67" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
       <c r="I67" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J67" s="14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A68" s="22"/>
-      <c r="B68" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D68" s="12"/>
-      <c r="E68" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="F68" s="22"/>
-      <c r="G68" s="22"/>
-      <c r="H68" s="22"/>
-      <c r="I68" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="J68" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K68" s="12"/>
-      <c r="L68" s="27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A69" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B69" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D69" s="12"/>
-      <c r="E69" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="F69" s="22"/>
-      <c r="G69" s="22"/>
-      <c r="H69" s="22"/>
-      <c r="I69" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="J69" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K69" s="12"/>
-      <c r="L69" s="12"/>
-    </row>
-    <row r="70" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A70" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B70" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="D70" s="12"/>
-      <c r="E70" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="F70" s="22"/>
-      <c r="G70" s="22"/>
-      <c r="H70" s="22"/>
-      <c r="I70" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="J70" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K70" s="12"/>
-      <c r="L70" s="12"/>
-    </row>
-    <row r="71" spans="1:12" s="14" customFormat="1">
-      <c r="A71" s="15" t="s">
-        <v>185</v>
-      </c>
-      <c r="B71" s="16"/>
-      <c r="C71" s="16"/>
-      <c r="D71" s="16"/>
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="16"/>
-      <c r="H71" s="16"/>
-      <c r="I71" s="16"/>
-      <c r="J71" s="16"/>
-      <c r="K71" s="16"/>
-      <c r="L71" s="16"/>
-    </row>
-    <row r="72" spans="1:12" s="14" customFormat="1">
-      <c r="A72" s="11"/>
+      <c r="J67" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="B68" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C68" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J68" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L68" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A69" s="11"/>
+      <c r="B69" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H69" s="11"/>
+      <c r="I69" s="11"/>
+      <c r="J69" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A70" s="11"/>
+      <c r="B70" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H70" s="11"/>
+      <c r="I70" s="11"/>
+      <c r="J70" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" s="13" customFormat="1" ht="45">
+      <c r="A71" s="11"/>
+      <c r="B71" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C71" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H71" s="11"/>
+      <c r="I71" s="11"/>
+      <c r="J71" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A72" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="B72" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="6" t="s">
-        <v>190</v>
+        <v>71</v>
+      </c>
+      <c r="C72" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>178</v>
       </c>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
       <c r="H72" s="11"/>
       <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
-      <c r="L72" s="11"/>
-    </row>
-    <row r="73" spans="1:12" s="14" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A73" s="11"/>
-      <c r="B73" s="7" t="s">
+      <c r="J72" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" s="32" customFormat="1" ht="30">
+      <c r="A73" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B73" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
+      <c r="I73" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="J73" s="32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" s="30" customFormat="1">
+      <c r="A74" s="34"/>
+      <c r="B74" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="E74" s="35"/>
+      <c r="F74" s="34"/>
+      <c r="G74" s="34"/>
+      <c r="H74" s="34"/>
+      <c r="I74" s="34"/>
+    </row>
+    <row r="75" spans="1:12" s="30" customFormat="1">
+      <c r="A75" s="34"/>
+      <c r="B75" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="E75" s="35"/>
+      <c r="F75" s="34"/>
+      <c r="G75" s="34"/>
+      <c r="H75" s="34"/>
+      <c r="I75" s="34"/>
+    </row>
+    <row r="76" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A76" s="21"/>
+      <c r="B76" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D76" s="12"/>
+      <c r="E76" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J76" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K76" s="12"/>
+      <c r="L76" s="26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" s="13" customFormat="1">
+      <c r="A77" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B77" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D77" s="12"/>
+      <c r="E77" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J77" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K77" s="12"/>
+      <c r="L77" s="12"/>
+    </row>
+    <row r="78" spans="1:12" s="13" customFormat="1">
+      <c r="A78" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="C78" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D78" s="12"/>
+      <c r="E78" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="F78" s="21"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J78" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+    </row>
+    <row r="79" spans="1:12" s="13" customFormat="1" ht="30">
+      <c r="A79" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15"/>
+      <c r="D79" s="15"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+    </row>
+    <row r="80" spans="1:12" s="30" customFormat="1">
+      <c r="A80" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="E80" s="29"/>
+      <c r="F80" s="34"/>
+      <c r="G80" s="34"/>
+      <c r="H80" s="34"/>
+      <c r="I80" s="34"/>
+      <c r="L80" s="35"/>
+    </row>
+    <row r="81" spans="1:12" s="30" customFormat="1">
+      <c r="A81" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="E81" s="29"/>
+      <c r="F81" s="34"/>
+      <c r="G81" s="34"/>
+      <c r="H81" s="34"/>
+      <c r="I81" s="34"/>
+      <c r="L81" s="35"/>
+    </row>
+    <row r="82" spans="1:12" s="30" customFormat="1">
+      <c r="A82" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="E82" s="29"/>
+      <c r="F82" s="34"/>
+      <c r="G82" s="34"/>
+      <c r="H82" s="34"/>
+      <c r="I82" s="34"/>
+      <c r="L82" s="35"/>
+    </row>
+    <row r="83" spans="1:12" s="30" customFormat="1">
+      <c r="A83" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="E83" s="29"/>
+      <c r="F83" s="34"/>
+      <c r="G83" s="34"/>
+      <c r="H83" s="34"/>
+      <c r="I83" s="34"/>
+      <c r="L83" s="35"/>
+    </row>
+    <row r="84" spans="1:12" s="30" customFormat="1">
+      <c r="A84" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="E84" s="29"/>
+      <c r="F84" s="34"/>
+      <c r="G84" s="34"/>
+      <c r="H84" s="34"/>
+      <c r="I84" s="34"/>
+      <c r="L84" s="35"/>
+    </row>
+    <row r="85" spans="1:12" s="30" customFormat="1">
+      <c r="A85" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="E85" s="29"/>
+      <c r="F85" s="34"/>
+      <c r="G85" s="34"/>
+      <c r="H85" s="34"/>
+      <c r="I85" s="34"/>
+      <c r="L85" s="35"/>
+    </row>
+    <row r="86" spans="1:12" s="13" customFormat="1">
+      <c r="A86" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B86" s="15"/>
+      <c r="C86" s="15"/>
+      <c r="D86" s="15"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+    </row>
+    <row r="87" spans="1:12" s="13" customFormat="1">
+      <c r="A87" s="11"/>
+      <c r="B87" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="F87" s="11"/>
+      <c r="G87" s="11"/>
+      <c r="H87" s="11"/>
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="11"/>
+      <c r="L87" s="11"/>
+    </row>
+    <row r="88" spans="1:12" s="13" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A88" s="11"/>
+      <c r="B88" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="E73" s="6" t="s">
+      <c r="E88" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="F73" s="7"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-    </row>
-    <row r="74" spans="1:12" s="14" customFormat="1">
-      <c r="A74" s="11"/>
-      <c r="E74" s="18"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-    </row>
-    <row r="75" spans="1:12" s="14" customFormat="1">
-      <c r="A75" s="11"/>
-      <c r="B75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-    </row>
-    <row r="76" spans="1:12" s="14" customFormat="1">
-      <c r="A76" s="11" t="s">
+      <c r="F88" s="7"/>
+      <c r="G88" s="11"/>
+      <c r="H88" s="11"/>
+    </row>
+    <row r="89" spans="1:12" s="13" customFormat="1">
+      <c r="A89" s="11"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="11"/>
+      <c r="G89" s="11"/>
+      <c r="H89" s="11"/>
+      <c r="I89" s="11"/>
+    </row>
+    <row r="90" spans="1:12" s="13" customFormat="1">
+      <c r="A90" s="11"/>
+      <c r="B90" s="11"/>
+      <c r="E90" s="11"/>
+      <c r="F90" s="11"/>
+      <c r="G90" s="11"/>
+      <c r="H90" s="11"/>
+      <c r="I90" s="11"/>
+    </row>
+    <row r="91" spans="1:12" s="13" customFormat="1">
+      <c r="A91" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-    </row>
-    <row r="77" spans="1:12" s="14" customFormat="1" ht="60">
-      <c r="A77" s="11"/>
-      <c r="B77" s="11" t="s">
+      <c r="B91" s="11"/>
+      <c r="E91" s="11"/>
+      <c r="F91" s="11"/>
+      <c r="G91" s="11"/>
+      <c r="H91" s="11"/>
+      <c r="I91" s="11"/>
+    </row>
+    <row r="92" spans="1:12" s="13" customFormat="1" ht="60">
+      <c r="A92" s="11"/>
+      <c r="B92" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C77" s="14" t="s">
+      <c r="C92" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-    </row>
-    <row r="78" spans="1:12" s="14" customFormat="1">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-    </row>
-    <row r="79" spans="1:12" s="14" customFormat="1">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-    </row>
-    <row r="80" spans="1:12" s="14" customFormat="1">
-      <c r="A80" s="11"/>
-      <c r="B80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-    </row>
-    <row r="81" spans="1:9" s="14" customFormat="1">
-      <c r="A81" s="11"/>
-      <c r="B81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
-    </row>
-    <row r="82" spans="1:9" s="14" customFormat="1">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-    </row>
-    <row r="83" spans="1:9" s="14" customFormat="1">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="11"/>
-    </row>
-    <row r="84" spans="1:9">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-    </row>
-    <row r="85" spans="1:9">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-    </row>
-    <row r="86" spans="1:9">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-    </row>
-    <row r="87" spans="1:9">
-      <c r="A87" s="8"/>
-      <c r="B87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-    </row>
-    <row r="88" spans="1:9">
-      <c r="A88" s="8"/>
-      <c r="B88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
-    </row>
-    <row r="89" spans="1:9">
-      <c r="A89" s="8"/>
-      <c r="B89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-    </row>
-    <row r="90" spans="1:9">
-      <c r="A90" s="8"/>
-      <c r="B90" s="8"/>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="8"/>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
-    </row>
-    <row r="91" spans="1:9">
-      <c r="A91" s="8"/>
-      <c r="B91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-    </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="8"/>
-      <c r="B92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-    </row>
-    <row r="93" spans="1:9">
-      <c r="A93" s="8"/>
-      <c r="B93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-    </row>
-    <row r="94" spans="1:9">
-      <c r="A94" s="8"/>
-      <c r="B94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-    </row>
-    <row r="95" spans="1:9">
-      <c r="A95" s="8"/>
-      <c r="B95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-    </row>
-    <row r="96" spans="1:9">
-      <c r="A96" s="8"/>
-      <c r="B96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-    </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="8"/>
-      <c r="B97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
-    </row>
-    <row r="98" spans="1:9">
-      <c r="A98" s="8"/>
-      <c r="B98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
+      <c r="E92" s="11"/>
+      <c r="F92" s="11"/>
+      <c r="G92" s="11"/>
+      <c r="H92" s="11"/>
+      <c r="I92" s="11"/>
+    </row>
+    <row r="93" spans="1:12" s="13" customFormat="1">
+      <c r="A93" s="11"/>
+      <c r="B93" s="11"/>
+      <c r="E93" s="11"/>
+      <c r="F93" s="11"/>
+      <c r="G93" s="11"/>
+      <c r="H93" s="11"/>
+      <c r="I93" s="11"/>
+    </row>
+    <row r="94" spans="1:12" s="13" customFormat="1">
+      <c r="A94" s="11"/>
+      <c r="B94" s="11"/>
+      <c r="E94" s="11"/>
+      <c r="F94" s="11"/>
+      <c r="G94" s="11"/>
+      <c r="H94" s="11"/>
+      <c r="I94" s="11"/>
+    </row>
+    <row r="95" spans="1:12" s="13" customFormat="1">
+      <c r="A95" s="11"/>
+      <c r="B95" s="11"/>
+      <c r="E95" s="11"/>
+      <c r="F95" s="11"/>
+      <c r="G95" s="11"/>
+      <c r="H95" s="11"/>
+      <c r="I95" s="11"/>
+    </row>
+    <row r="96" spans="1:12" s="13" customFormat="1">
+      <c r="A96" s="11"/>
+      <c r="B96" s="11"/>
+      <c r="E96" s="11"/>
+      <c r="F96" s="11"/>
+      <c r="G96" s="11"/>
+      <c r="H96" s="11"/>
+      <c r="I96" s="11"/>
+    </row>
+    <row r="97" spans="1:9" s="13" customFormat="1">
+      <c r="A97" s="11"/>
+      <c r="B97" s="11"/>
+      <c r="E97" s="11"/>
+      <c r="F97" s="11"/>
+      <c r="G97" s="11"/>
+      <c r="H97" s="11"/>
+      <c r="I97" s="11"/>
+    </row>
+    <row r="98" spans="1:9" s="13" customFormat="1">
+      <c r="A98" s="11"/>
+      <c r="B98" s="11"/>
+      <c r="E98" s="11"/>
+      <c r="F98" s="11"/>
+      <c r="G98" s="11"/>
+      <c r="H98" s="11"/>
+      <c r="I98" s="11"/>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="8"/>
@@ -6194,7 +6368,7 @@
       <c r="H275" s="8"/>
       <c r="I275" s="8"/>
     </row>
-    <row r="276" spans="1:9" hidden="1">
+    <row r="276" spans="1:9">
       <c r="A276" s="8"/>
       <c r="B276" s="8"/>
       <c r="E276" s="8"/>
@@ -6203,7 +6377,7 @@
       <c r="H276" s="8"/>
       <c r="I276" s="8"/>
     </row>
-    <row r="277" spans="1:9" hidden="1">
+    <row r="277" spans="1:9">
       <c r="A277" s="8"/>
       <c r="B277" s="8"/>
       <c r="E277" s="8"/>
@@ -6212,7 +6386,7 @@
       <c r="H277" s="8"/>
       <c r="I277" s="8"/>
     </row>
-    <row r="278" spans="1:9" hidden="1">
+    <row r="278" spans="1:9">
       <c r="A278" s="8"/>
       <c r="B278" s="8"/>
       <c r="E278" s="8"/>
@@ -6221,7 +6395,7 @@
       <c r="H278" s="8"/>
       <c r="I278" s="8"/>
     </row>
-    <row r="279" spans="1:9" hidden="1">
+    <row r="279" spans="1:9">
       <c r="A279" s="8"/>
       <c r="B279" s="8"/>
       <c r="E279" s="8"/>
@@ -6230,7 +6404,7 @@
       <c r="H279" s="8"/>
       <c r="I279" s="8"/>
     </row>
-    <row r="280" spans="1:9" hidden="1">
+    <row r="280" spans="1:9">
       <c r="A280" s="8"/>
       <c r="B280" s="8"/>
       <c r="E280" s="8"/>
@@ -6239,7 +6413,7 @@
       <c r="H280" s="8"/>
       <c r="I280" s="8"/>
     </row>
-    <row r="281" spans="1:9" hidden="1">
+    <row r="281" spans="1:9">
       <c r="A281" s="8"/>
       <c r="B281" s="8"/>
       <c r="E281" s="8"/>
@@ -6248,7 +6422,7 @@
       <c r="H281" s="8"/>
       <c r="I281" s="8"/>
     </row>
-    <row r="282" spans="1:9" hidden="1">
+    <row r="282" spans="1:9">
       <c r="A282" s="8"/>
       <c r="B282" s="8"/>
       <c r="E282" s="8"/>
@@ -6257,7 +6431,7 @@
       <c r="H282" s="8"/>
       <c r="I282" s="8"/>
     </row>
-    <row r="283" spans="1:9" hidden="1">
+    <row r="283" spans="1:9">
       <c r="A283" s="8"/>
       <c r="B283" s="8"/>
       <c r="E283" s="8"/>
@@ -6266,7 +6440,7 @@
       <c r="H283" s="8"/>
       <c r="I283" s="8"/>
     </row>
-    <row r="284" spans="1:9" hidden="1">
+    <row r="284" spans="1:9">
       <c r="A284" s="8"/>
       <c r="B284" s="8"/>
       <c r="E284" s="8"/>
@@ -6275,7 +6449,7 @@
       <c r="H284" s="8"/>
       <c r="I284" s="8"/>
     </row>
-    <row r="285" spans="1:9" hidden="1">
+    <row r="285" spans="1:9">
       <c r="A285" s="8"/>
       <c r="B285" s="8"/>
       <c r="E285" s="8"/>
@@ -6284,7 +6458,7 @@
       <c r="H285" s="8"/>
       <c r="I285" s="8"/>
     </row>
-    <row r="286" spans="1:9" hidden="1">
+    <row r="286" spans="1:9">
       <c r="A286" s="8"/>
       <c r="B286" s="8"/>
       <c r="E286" s="8"/>
@@ -6293,7 +6467,7 @@
       <c r="H286" s="8"/>
       <c r="I286" s="8"/>
     </row>
-    <row r="287" spans="1:9" hidden="1">
+    <row r="287" spans="1:9">
       <c r="A287" s="8"/>
       <c r="B287" s="8"/>
       <c r="E287" s="8"/>
@@ -6302,7 +6476,7 @@
       <c r="H287" s="8"/>
       <c r="I287" s="8"/>
     </row>
-    <row r="288" spans="1:9" hidden="1">
+    <row r="288" spans="1:9">
       <c r="A288" s="8"/>
       <c r="B288" s="8"/>
       <c r="E288" s="8"/>
@@ -6311,7 +6485,7 @@
       <c r="H288" s="8"/>
       <c r="I288" s="8"/>
     </row>
-    <row r="289" spans="1:9" hidden="1">
+    <row r="289" spans="1:9">
       <c r="A289" s="8"/>
       <c r="B289" s="8"/>
       <c r="E289" s="8"/>
@@ -6329,7 +6503,7 @@
       <c r="H290" s="8"/>
       <c r="I290" s="8"/>
     </row>
-    <row r="291" spans="1:9">
+    <row r="291" spans="1:9" hidden="1">
       <c r="A291" s="8"/>
       <c r="B291" s="8"/>
       <c r="E291" s="8"/>
@@ -6338,7 +6512,7 @@
       <c r="H291" s="8"/>
       <c r="I291" s="8"/>
     </row>
-    <row r="292" spans="1:9">
+    <row r="292" spans="1:9" hidden="1">
       <c r="A292" s="8"/>
       <c r="B292" s="8"/>
       <c r="E292" s="8"/>
@@ -6347,7 +6521,7 @@
       <c r="H292" s="8"/>
       <c r="I292" s="8"/>
     </row>
-    <row r="293" spans="1:9">
+    <row r="293" spans="1:9" hidden="1">
       <c r="A293" s="8"/>
       <c r="B293" s="8"/>
       <c r="E293" s="8"/>
@@ -6356,7 +6530,7 @@
       <c r="H293" s="8"/>
       <c r="I293" s="8"/>
     </row>
-    <row r="294" spans="1:9">
+    <row r="294" spans="1:9" hidden="1">
       <c r="A294" s="8"/>
       <c r="B294" s="8"/>
       <c r="E294" s="8"/>
@@ -6365,7 +6539,7 @@
       <c r="H294" s="8"/>
       <c r="I294" s="8"/>
     </row>
-    <row r="295" spans="1:9">
+    <row r="295" spans="1:9" hidden="1">
       <c r="A295" s="8"/>
       <c r="B295" s="8"/>
       <c r="E295" s="8"/>
@@ -6374,7 +6548,7 @@
       <c r="H295" s="8"/>
       <c r="I295" s="8"/>
     </row>
-    <row r="296" spans="1:9">
+    <row r="296" spans="1:9" hidden="1">
       <c r="A296" s="8"/>
       <c r="B296" s="8"/>
       <c r="E296" s="8"/>
@@ -6383,7 +6557,7 @@
       <c r="H296" s="8"/>
       <c r="I296" s="8"/>
     </row>
-    <row r="297" spans="1:9">
+    <row r="297" spans="1:9" hidden="1">
       <c r="A297" s="8"/>
       <c r="B297" s="8"/>
       <c r="E297" s="8"/>
@@ -6392,7 +6566,7 @@
       <c r="H297" s="8"/>
       <c r="I297" s="8"/>
     </row>
-    <row r="298" spans="1:9">
+    <row r="298" spans="1:9" hidden="1">
       <c r="A298" s="8"/>
       <c r="B298" s="8"/>
       <c r="E298" s="8"/>
@@ -6401,7 +6575,7 @@
       <c r="H298" s="8"/>
       <c r="I298" s="8"/>
     </row>
-    <row r="299" spans="1:9">
+    <row r="299" spans="1:9" hidden="1">
       <c r="A299" s="8"/>
       <c r="B299" s="8"/>
       <c r="E299" s="8"/>
@@ -6410,7 +6584,7 @@
       <c r="H299" s="8"/>
       <c r="I299" s="8"/>
     </row>
-    <row r="300" spans="1:9">
+    <row r="300" spans="1:9" hidden="1">
       <c r="A300" s="8"/>
       <c r="B300" s="8"/>
       <c r="E300" s="8"/>
@@ -6419,7 +6593,7 @@
       <c r="H300" s="8"/>
       <c r="I300" s="8"/>
     </row>
-    <row r="301" spans="1:9">
+    <row r="301" spans="1:9" hidden="1">
       <c r="A301" s="8"/>
       <c r="B301" s="8"/>
       <c r="E301" s="8"/>
@@ -6428,7 +6602,7 @@
       <c r="H301" s="8"/>
       <c r="I301" s="8"/>
     </row>
-    <row r="302" spans="1:9">
+    <row r="302" spans="1:9" hidden="1">
       <c r="A302" s="8"/>
       <c r="B302" s="8"/>
       <c r="E302" s="8"/>
@@ -6437,7 +6611,7 @@
       <c r="H302" s="8"/>
       <c r="I302" s="8"/>
     </row>
-    <row r="303" spans="1:9">
+    <row r="303" spans="1:9" hidden="1">
       <c r="A303" s="8"/>
       <c r="B303" s="8"/>
       <c r="E303" s="8"/>
@@ -6446,7 +6620,7 @@
       <c r="H303" s="8"/>
       <c r="I303" s="8"/>
     </row>
-    <row r="304" spans="1:9">
+    <row r="304" spans="1:9" hidden="1">
       <c r="A304" s="8"/>
       <c r="B304" s="8"/>
       <c r="E304" s="8"/>
@@ -7201,6 +7375,141 @@
       <c r="G387" s="8"/>
       <c r="H387" s="8"/>
       <c r="I387" s="8"/>
+    </row>
+    <row r="388" spans="1:9">
+      <c r="A388" s="8"/>
+      <c r="B388" s="8"/>
+      <c r="E388" s="8"/>
+      <c r="F388" s="8"/>
+      <c r="G388" s="8"/>
+      <c r="H388" s="8"/>
+      <c r="I388" s="8"/>
+    </row>
+    <row r="389" spans="1:9">
+      <c r="A389" s="8"/>
+      <c r="B389" s="8"/>
+      <c r="E389" s="8"/>
+      <c r="F389" s="8"/>
+      <c r="G389" s="8"/>
+      <c r="H389" s="8"/>
+      <c r="I389" s="8"/>
+    </row>
+    <row r="390" spans="1:9">
+      <c r="A390" s="8"/>
+      <c r="B390" s="8"/>
+      <c r="E390" s="8"/>
+      <c r="F390" s="8"/>
+      <c r="G390" s="8"/>
+      <c r="H390" s="8"/>
+      <c r="I390" s="8"/>
+    </row>
+    <row r="391" spans="1:9">
+      <c r="A391" s="8"/>
+      <c r="B391" s="8"/>
+      <c r="E391" s="8"/>
+      <c r="F391" s="8"/>
+      <c r="G391" s="8"/>
+      <c r="H391" s="8"/>
+      <c r="I391" s="8"/>
+    </row>
+    <row r="392" spans="1:9">
+      <c r="A392" s="8"/>
+      <c r="B392" s="8"/>
+      <c r="E392" s="8"/>
+      <c r="F392" s="8"/>
+      <c r="G392" s="8"/>
+      <c r="H392" s="8"/>
+      <c r="I392" s="8"/>
+    </row>
+    <row r="393" spans="1:9">
+      <c r="A393" s="8"/>
+      <c r="B393" s="8"/>
+      <c r="E393" s="8"/>
+      <c r="F393" s="8"/>
+      <c r="G393" s="8"/>
+      <c r="H393" s="8"/>
+      <c r="I393" s="8"/>
+    </row>
+    <row r="394" spans="1:9">
+      <c r="A394" s="8"/>
+      <c r="B394" s="8"/>
+      <c r="E394" s="8"/>
+      <c r="F394" s="8"/>
+      <c r="G394" s="8"/>
+      <c r="H394" s="8"/>
+      <c r="I394" s="8"/>
+    </row>
+    <row r="395" spans="1:9">
+      <c r="A395" s="8"/>
+      <c r="B395" s="8"/>
+      <c r="E395" s="8"/>
+      <c r="F395" s="8"/>
+      <c r="G395" s="8"/>
+      <c r="H395" s="8"/>
+      <c r="I395" s="8"/>
+    </row>
+    <row r="396" spans="1:9">
+      <c r="A396" s="8"/>
+      <c r="B396" s="8"/>
+      <c r="E396" s="8"/>
+      <c r="F396" s="8"/>
+      <c r="G396" s="8"/>
+      <c r="H396" s="8"/>
+      <c r="I396" s="8"/>
+    </row>
+    <row r="397" spans="1:9">
+      <c r="A397" s="8"/>
+      <c r="B397" s="8"/>
+      <c r="E397" s="8"/>
+      <c r="F397" s="8"/>
+      <c r="G397" s="8"/>
+      <c r="H397" s="8"/>
+      <c r="I397" s="8"/>
+    </row>
+    <row r="398" spans="1:9">
+      <c r="A398" s="8"/>
+      <c r="B398" s="8"/>
+      <c r="E398" s="8"/>
+      <c r="F398" s="8"/>
+      <c r="G398" s="8"/>
+      <c r="H398" s="8"/>
+      <c r="I398" s="8"/>
+    </row>
+    <row r="399" spans="1:9">
+      <c r="A399" s="8"/>
+      <c r="B399" s="8"/>
+      <c r="E399" s="8"/>
+      <c r="F399" s="8"/>
+      <c r="G399" s="8"/>
+      <c r="H399" s="8"/>
+      <c r="I399" s="8"/>
+    </row>
+    <row r="400" spans="1:9">
+      <c r="A400" s="8"/>
+      <c r="B400" s="8"/>
+      <c r="E400" s="8"/>
+      <c r="F400" s="8"/>
+      <c r="G400" s="8"/>
+      <c r="H400" s="8"/>
+      <c r="I400" s="8"/>
+    </row>
+    <row r="401" spans="1:9">
+      <c r="A401" s="8"/>
+      <c r="B401" s="8"/>
+      <c r="E401" s="8"/>
+      <c r="F401" s="8"/>
+      <c r="G401" s="8"/>
+      <c r="H401" s="8"/>
+      <c r="I401" s="8"/>
+    </row>
+    <row r="402" spans="1:9">
+      <c r="A402" s="8"/>
+      <c r="B402" s="8"/>
+      <c r="E402" s="8"/>
+      <c r="F402" s="8"/>
+      <c r="G402" s="8"/>
+      <c r="H402" s="8"/>
+      <c r="I402" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Broke out Arrest location fields in detail.
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReportMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Booking_Reporting/artifacts/service_model/information_model/IEPD/documentation/BookingReportMapping.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="216">
   <si>
     <t>Race</t>
   </si>
@@ -664,13 +664,16 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>ADD LOCATION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -759,6 +762,11 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1583,7 +1591,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1661,9 +1669,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1687,6 +1692,24 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="766">
@@ -2792,8 +2815,8 @@
   <dimension ref="A1:L402"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A83" sqref="A83:XFD85"/>
+      <pane ySplit="2" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2812,10 +2835,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="9"/>
       <c r="D1" s="10"/>
       <c r="E1" s="1"/>
@@ -3045,103 +3068,103 @@
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
     </row>
-    <row r="13" spans="1:12" s="30" customFormat="1">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29" t="s">
+    <row r="13" spans="1:12" s="29" customFormat="1">
+      <c r="A13" s="27"/>
+      <c r="B13" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-    </row>
-    <row r="14" spans="1:12" s="30" customFormat="1">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+    </row>
+    <row r="14" spans="1:12" s="29" customFormat="1">
+      <c r="A14" s="27"/>
+      <c r="B14" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-    </row>
-    <row r="15" spans="1:12" s="30" customFormat="1">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+    </row>
+    <row r="15" spans="1:12" s="29" customFormat="1">
+      <c r="A15" s="27"/>
+      <c r="B15" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-    </row>
-    <row r="16" spans="1:12" s="30" customFormat="1">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29" t="s">
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+    </row>
+    <row r="16" spans="1:12" s="29" customFormat="1">
+      <c r="A16" s="27"/>
+      <c r="B16" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-    </row>
-    <row r="17" spans="1:12" s="30" customFormat="1">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29" t="s">
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+    </row>
+    <row r="17" spans="1:12" s="29" customFormat="1">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-    </row>
-    <row r="18" spans="1:12" s="30" customFormat="1">
-      <c r="A18" s="28"/>
-      <c r="B18" s="29" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+    </row>
+    <row r="18" spans="1:12" s="29" customFormat="1">
+      <c r="A18" s="27"/>
+      <c r="B18" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="D18" s="29"/>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
     </row>
     <row r="19" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A19" s="6"/>
@@ -4117,29 +4140,31 @@
       <c r="K58" s="15"/>
       <c r="L58" s="15"/>
     </row>
-    <row r="59" spans="1:12" s="13" customFormat="1" ht="60">
-      <c r="A59" s="21"/>
-      <c r="B59" s="25" t="s">
+    <row r="59" spans="1:12" s="40" customFormat="1" ht="60">
+      <c r="A59" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="B59" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="12" t="s">
+      <c r="C59" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="12"/>
-      <c r="E59" s="7" t="s">
+      <c r="D59" s="38"/>
+      <c r="E59" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="F59" s="12"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="J59" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="K59" s="12"/>
-      <c r="L59" s="12"/>
+      <c r="F59" s="38"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="K59" s="38"/>
+      <c r="L59" s="38"/>
     </row>
     <row r="60" spans="1:12" s="13" customFormat="1" ht="45">
       <c r="A60" s="21"/>
@@ -4428,50 +4453,50 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:12" s="32" customFormat="1" ht="30">
-      <c r="A73" s="31" t="s">
+    <row r="73" spans="1:12" s="31" customFormat="1" ht="30">
+      <c r="A73" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="B73" s="32" t="s">
+      <c r="B73" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C73" s="32" t="s">
+      <c r="C73" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="33" t="s">
+      <c r="E73" s="32" t="s">
         <v>179</v>
       </c>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="31"/>
-      <c r="I73" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="J73" s="32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" s="30" customFormat="1">
-      <c r="A74" s="34"/>
-      <c r="B74" s="30" t="s">
+      <c r="F73" s="30"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="30"/>
+      <c r="I73" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="J73" s="31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" s="29" customFormat="1">
+      <c r="A74" s="33"/>
+      <c r="B74" s="29" t="s">
         <v>205</v>
       </c>
-      <c r="E74" s="35"/>
-      <c r="F74" s="34"/>
-      <c r="G74" s="34"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="34"/>
-    </row>
-    <row r="75" spans="1:12" s="30" customFormat="1">
-      <c r="A75" s="34"/>
-      <c r="B75" s="30" t="s">
+      <c r="E74" s="34"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="33"/>
+      <c r="H74" s="33"/>
+      <c r="I74" s="33"/>
+    </row>
+    <row r="75" spans="1:12" s="29" customFormat="1">
+      <c r="A75" s="33"/>
+      <c r="B75" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="E75" s="35"/>
-      <c r="F75" s="34"/>
-      <c r="G75" s="34"/>
-      <c r="H75" s="34"/>
-      <c r="I75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="33"/>
+      <c r="I75" s="33"/>
     </row>
     <row r="76" spans="1:12" s="13" customFormat="1" ht="30">
       <c r="A76" s="21"/>
@@ -4567,71 +4592,71 @@
       <c r="K79" s="15"/>
       <c r="L79" s="15"/>
     </row>
-    <row r="80" spans="1:12" s="30" customFormat="1">
-      <c r="A80" s="34" t="s">
+    <row r="80" spans="1:12" s="29" customFormat="1">
+      <c r="A80" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="E80" s="29"/>
-      <c r="F80" s="34"/>
-      <c r="G80" s="34"/>
-      <c r="H80" s="34"/>
-      <c r="I80" s="34"/>
-      <c r="L80" s="35"/>
-    </row>
-    <row r="81" spans="1:12" s="30" customFormat="1">
-      <c r="A81" s="34" t="s">
+      <c r="E80" s="28"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="33"/>
+      <c r="H80" s="33"/>
+      <c r="I80" s="33"/>
+      <c r="L80" s="34"/>
+    </row>
+    <row r="81" spans="1:12" s="29" customFormat="1">
+      <c r="A81" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="E81" s="29"/>
-      <c r="F81" s="34"/>
-      <c r="G81" s="34"/>
-      <c r="H81" s="34"/>
-      <c r="I81" s="34"/>
-      <c r="L81" s="35"/>
-    </row>
-    <row r="82" spans="1:12" s="30" customFormat="1">
-      <c r="A82" s="34" t="s">
+      <c r="E81" s="28"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="33"/>
+      <c r="I81" s="33"/>
+      <c r="L81" s="34"/>
+    </row>
+    <row r="82" spans="1:12" s="29" customFormat="1">
+      <c r="A82" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="E82" s="29"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="34"/>
-      <c r="H82" s="34"/>
-      <c r="I82" s="34"/>
-      <c r="L82" s="35"/>
-    </row>
-    <row r="83" spans="1:12" s="30" customFormat="1">
-      <c r="A83" s="34" t="s">
+      <c r="E82" s="28"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="33"/>
+      <c r="H82" s="33"/>
+      <c r="I82" s="33"/>
+      <c r="L82" s="34"/>
+    </row>
+    <row r="83" spans="1:12" s="29" customFormat="1">
+      <c r="A83" s="33" t="s">
         <v>211</v>
       </c>
-      <c r="E83" s="29"/>
-      <c r="F83" s="34"/>
-      <c r="G83" s="34"/>
-      <c r="H83" s="34"/>
-      <c r="I83" s="34"/>
-      <c r="L83" s="35"/>
-    </row>
-    <row r="84" spans="1:12" s="30" customFormat="1">
-      <c r="A84" s="34" t="s">
+      <c r="E83" s="28"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="33"/>
+      <c r="H83" s="33"/>
+      <c r="I83" s="33"/>
+      <c r="L83" s="34"/>
+    </row>
+    <row r="84" spans="1:12" s="29" customFormat="1">
+      <c r="A84" s="33" t="s">
         <v>212</v>
       </c>
-      <c r="E84" s="29"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="34"/>
-      <c r="H84" s="34"/>
-      <c r="I84" s="34"/>
-      <c r="L84" s="35"/>
-    </row>
-    <row r="85" spans="1:12" s="30" customFormat="1">
-      <c r="A85" s="34" t="s">
+      <c r="E84" s="28"/>
+      <c r="F84" s="33"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="33"/>
+      <c r="I84" s="33"/>
+      <c r="L84" s="34"/>
+    </row>
+    <row r="85" spans="1:12" s="29" customFormat="1">
+      <c r="A85" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="E85" s="29"/>
-      <c r="F85" s="34"/>
-      <c r="G85" s="34"/>
-      <c r="H85" s="34"/>
-      <c r="I85" s="34"/>
-      <c r="L85" s="35"/>
+      <c r="E85" s="28"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="33"/>
+      <c r="H85" s="33"/>
+      <c r="I85" s="33"/>
+      <c r="L85" s="34"/>
     </row>
     <row r="86" spans="1:12" s="13" customFormat="1">
       <c r="A86" s="14" t="s">

</xml_diff>